<commit_message>
final code for newtours
</commit_message>
<xml_diff>
--- a/src/main/java/abc.xlsx
+++ b/src/main/java/abc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14895" windowHeight="1995" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14895" windowHeight="2715" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginexcel" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="bookflightexcel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O5"/>
+  <oleSize ref="A1:O7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>demo</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>BANGLADESH</t>
+  </si>
+  <si>
+    <t>afreen</t>
+  </si>
+  <si>
+    <t>rahman</t>
   </si>
 </sst>
 </file>
@@ -425,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -468,15 +474,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -487,42 +493,51 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1">
+      <c r="H1">
         <v>45534258</v>
       </c>
-      <c r="F1">
+      <c r="I1">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="J1">
         <v>2008</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="R1">
         <v>1216</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>